<commit_message>
add a grid frequency file
1. 增加一個沒有緊急狀態的頻率表
</commit_message>
<xml_diff>
--- a/schedule_Edreg.xlsx
+++ b/schedule_Edreg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\使用者\Desktop\高國鈞\Github\Project_EdReg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933438AD-1644-43AE-8ED0-FBB1F9E634E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472AEA4D-B69E-4D00-A93C-C2A3C6441DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15720" xr2:uid="{349B18BF-DA2C-4AD6-9CC8-FAB259AD76CA}"/>
   </bookViews>
@@ -417,8 +417,8 @@
   <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -673,7 +673,7 @@
         <v>0.60416666666666652</v>
       </c>
       <c r="B28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -745,7 +745,7 @@
         <v>0.68749999999999956</v>
       </c>
       <c r="B36" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>